<commit_message>
Updating posts, adding Schwab callback URL
</commit_message>
<xml_diff>
--- a/Data_Manual/VIX_Transactions_Brokerage.xlsx
+++ b/Data_Manual/VIX_Transactions_Brokerage.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="131">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -52,12 +52,69 @@
     <t xml:space="preserve">Comments</t>
   </si>
   <si>
+    <t xml:space="preserve">05/12/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sell to Close</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VIX 06/18/2025 45.00 P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUT CBOE VOLATILITY IDX $45 EXP 06/18/25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$25.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$2.16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$4997.84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Market up on positive news of lowering tariffs with China; VIX down 15%, VVIX down 10%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VIX 06/18/2025 27.00 P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUT CBOE VOLATILITY IDX $27 EXP 06/18/25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$7.55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$6.49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$4523.51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VIX 06/18/2025 36.00 P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUT CBOE VOLATILITY IDX $36 EXP 06/18/25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$16.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$3.24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$4796.76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$7.40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$4433.51</t>
+  </si>
+  <si>
     <t xml:space="preserve">05/07/2025</t>
   </si>
   <si>
-    <t xml:space="preserve">Sell to Close</t>
-  </si>
-  <si>
     <t xml:space="preserve">VIX 05/21/2025 26.00 P</t>
   </si>
   <si>
@@ -85,9 +142,6 @@
     <t xml:space="preserve">$13.75</t>
   </si>
   <si>
-    <t xml:space="preserve">$3.24</t>
-  </si>
-  <si>
     <t xml:space="preserve">$4121.76</t>
   </si>
   <si>
@@ -124,12 +178,6 @@
     <t xml:space="preserve">Buy to Open</t>
   </si>
   <si>
-    <t xml:space="preserve">VIX 06/18/2025 27.00 P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PUT CBOE VOLATILITY IDX $27 EXP 06/18/25</t>
-  </si>
-  <si>
     <t xml:space="preserve">$4.55</t>
   </si>
   <si>
@@ -151,9 +199,6 @@
     <t xml:space="preserve">$21.75</t>
   </si>
   <si>
-    <t xml:space="preserve">$2.16</t>
-  </si>
-  <si>
     <t xml:space="preserve">-$4352.16</t>
   </si>
   <si>
@@ -169,12 +214,6 @@
     <t xml:space="preserve">-$4312.16</t>
   </si>
   <si>
-    <t xml:space="preserve">VIX 06/18/2025 45.00 P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PUT CBOE VOLATILITY IDX $45 EXP 06/18/25</t>
-  </si>
-  <si>
     <t xml:space="preserve">$18.85</t>
   </si>
   <si>
@@ -209,12 +248,6 @@
   </si>
   <si>
     <t xml:space="preserve">-$3963.24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VIX 06/18/2025 36.00 P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PUT CBOE VOLATILITY IDX $36 EXP 06/18/25</t>
   </si>
   <si>
     <t xml:space="preserve">$13.40</t>
@@ -390,12 +423,11 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -411,6 +443,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Roboto"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -460,15 +498,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -595,24 +633,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="41.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="7.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="70.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="38.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="9.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="71.55"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -628,16 +665,16 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -661,7 +698,7 @@
         <v>13</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>14</v>
@@ -672,10 +709,8 @@
       <c r="H2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="2" t="n">
-        <v>24.47</v>
-      </c>
-      <c r="J2" s="2" t="s">
+      <c r="I2" s="1"/>
+      <c r="J2" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -693,7 +728,7 @@
         <v>19</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>20</v>
@@ -704,635 +739,645 @@
       <c r="H3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="2" t="n">
-        <v>24.51</v>
-      </c>
-      <c r="J3" s="2" t="s">
+      <c r="I3" s="1"/>
+      <c r="J3" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>28</v>
       </c>
       <c r="G5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2" t="s">
-        <v>31</v>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>4</v>
       </c>
       <c r="F6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="2" t="n">
+        <v>24.47</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="G7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
+      <c r="I7" s="2" t="n">
+        <v>24.51</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+      <c r="J8" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="F11" s="3" t="s">
+      <c r="G11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="E12" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>63</v>
+        <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="F13" s="3" t="s">
+      <c r="G13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>66</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="G14" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="H14" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="H14" s="3" t="s">
-        <v>72</v>
-      </c>
       <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
+      <c r="J14" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>34</v>
+        <v>70</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="E15" s="1" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F15" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>75</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="E16" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="E17" s="1" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="I17" s="2"/>
-      <c r="J17" s="2" t="s">
-        <v>84</v>
-      </c>
+      <c r="J17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="E18" s="1" t="n">
         <v>5</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>89</v>
+        <v>18</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>90</v>
+        <v>19</v>
       </c>
       <c r="E19" s="1" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="E20" s="1" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>43</v>
+        <v>82</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>100</v>
+        <v>31</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>101</v>
+        <v>32</v>
       </c>
       <c r="E21" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
+      <c r="J21" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="E22" s="1" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="E23" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>43</v>
+        <v>103</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="E24" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="E25" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -1342,13 +1387,13 @@
         <v>115</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="E26" s="1" t="n">
         <v>1</v>
@@ -1357,13 +1402,125 @@
         <v>118</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>119</v>
       </c>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E28" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E29" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E30" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Updating posts and scss
</commit_message>
<xml_diff>
--- a/Data_Manual/VIX_Transactions_Brokerage.xlsx
+++ b/Data_Manual/VIX_Transactions_Brokerage.xlsx
@@ -46,7 +46,7 @@
     <t xml:space="preserve">Amount</t>
   </si>
   <si>
-    <t xml:space="preserve">VIX_Level</t>
+    <t xml:space="preserve">Approx_VIX_Level</t>
   </si>
   <si>
     <t xml:space="preserve">Comments</t>
@@ -672,7 +672,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
+      <selection pane="topLeft" activeCell="F29" activeCellId="0" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -684,7 +684,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="6.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="9.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="15.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="71.55"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="11" style="1" width="11.53"/>
   </cols>
@@ -1112,6 +1113,9 @@
       <c r="H14" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="I14" s="1" t="n">
+        <v>22.73</v>
+      </c>
       <c r="J14" s="1" t="s">
         <v>66</v>
       </c>
@@ -1141,6 +1145,9 @@
       <c r="H15" s="2" t="s">
         <v>70</v>
       </c>
+      <c r="I15" s="1" t="n">
+        <v>27.37</v>
+      </c>
       <c r="J15" s="1" t="s">
         <v>71</v>
       </c>
@@ -1170,6 +1177,9 @@
       <c r="H16" s="2" t="s">
         <v>75</v>
       </c>
+      <c r="I16" s="1" t="n">
+        <v>55.44</v>
+      </c>
       <c r="J16" s="1" t="s">
         <v>76</v>
       </c>
@@ -1199,6 +1209,9 @@
       <c r="H17" s="2" t="s">
         <v>79</v>
       </c>
+      <c r="I17" s="1" t="n">
+        <v>49.07</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
@@ -1225,6 +1238,9 @@
       <c r="H18" s="2" t="s">
         <v>81</v>
       </c>
+      <c r="I18" s="1" t="n">
+        <v>46.17</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
@@ -1251,6 +1267,9 @@
       <c r="H19" s="2" t="s">
         <v>83</v>
       </c>
+      <c r="I19" s="1" t="n">
+        <v>53.65</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
@@ -1277,6 +1296,10 @@
       <c r="H20" s="2" t="s">
         <v>87</v>
       </c>
+      <c r="I20" s="1" t="n">
+        <f aca="false">(39.27+38.49)/2</f>
+        <v>38.88</v>
+      </c>
       <c r="J20" s="1" t="s">
         <v>76</v>
       </c>
@@ -1306,6 +1329,10 @@
       <c r="H21" s="2" t="s">
         <v>89</v>
       </c>
+      <c r="I21" s="1" t="n">
+        <f aca="false">(37.11+36.8)/2</f>
+        <v>36.955</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
@@ -1332,6 +1359,10 @@
       <c r="H22" s="2" t="s">
         <v>91</v>
       </c>
+      <c r="I22" s="1" t="n">
+        <f aca="false">(37.03+35.89)/2</f>
+        <v>36.46</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
@@ -1358,6 +1389,10 @@
       <c r="H23" s="2" t="s">
         <v>93</v>
       </c>
+      <c r="I23" s="1" t="n">
+        <f aca="false">(37.41+35.81)/2</f>
+        <v>36.61</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
@@ -1384,6 +1419,10 @@
       <c r="H24" s="2" t="s">
         <v>97</v>
       </c>
+      <c r="I24" s="1" t="n">
+        <f aca="false">(29.29+28.77)/2</f>
+        <v>29.03</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
@@ -1410,6 +1449,10 @@
       <c r="H25" s="2" t="s">
         <v>100</v>
       </c>
+      <c r="I25" s="1" t="n">
+        <f aca="false">(27.79+27.46)/2</f>
+        <v>27.625</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
@@ -1436,6 +1479,10 @@
       <c r="H26" s="2" t="s">
         <v>105</v>
       </c>
+      <c r="I26" s="1" t="n">
+        <f aca="false">(18.04+17.98)/2</f>
+        <v>18.01</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
@@ -1462,6 +1509,10 @@
       <c r="H27" s="2" t="s">
         <v>108</v>
       </c>
+      <c r="I27" s="1" t="n">
+        <f aca="false">(27.7+27.37)/2</f>
+        <v>27.535</v>
+      </c>
       <c r="J27" s="1" t="s">
         <v>109</v>
       </c>
@@ -1491,6 +1542,10 @@
       <c r="H28" s="2" t="s">
         <v>112</v>
       </c>
+      <c r="I28" s="1" t="n">
+        <f aca="false">(26.15+25.34)/2</f>
+        <v>25.745</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
@@ -1517,6 +1572,10 @@
       <c r="H29" s="2" t="s">
         <v>117</v>
       </c>
+      <c r="I29" s="1" t="n">
+        <f aca="false">(14.08+14.01)/2</f>
+        <v>14.045</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
@@ -1543,6 +1602,10 @@
       <c r="H30" s="2" t="s">
         <v>122</v>
       </c>
+      <c r="I30" s="1" t="n">
+        <f aca="false">(22.51+22.35)/2</f>
+        <v>22.43</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
@@ -1569,6 +1632,10 @@
       <c r="H31" s="2" t="s">
         <v>127</v>
       </c>
+      <c r="I31" s="1" t="n">
+        <f aca="false">(18.92+18.78)/2</f>
+        <v>18.85</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
@@ -1595,6 +1662,10 @@
       <c r="H32" s="2" t="s">
         <v>132</v>
       </c>
+      <c r="I32" s="1" t="n">
+        <f aca="false">(16.59+16.4)/2</f>
+        <v>16.495</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
@@ -1621,6 +1692,10 @@
       <c r="H33" s="2" t="s">
         <v>135</v>
       </c>
+      <c r="I33" s="1" t="n">
+        <f aca="false">(27.48+26.74)/2</f>
+        <v>27.11</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
@@ -1647,6 +1722,10 @@
       <c r="H34" s="2" t="s">
         <v>138</v>
       </c>
+      <c r="I34" s="1" t="n">
+        <f aca="false">(32.72+31.83)/2</f>
+        <v>32.275</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
@@ -1673,6 +1752,10 @@
       <c r="H35" s="2" t="s">
         <v>141</v>
       </c>
+      <c r="I35" s="1" t="n">
+        <f aca="false">(34.61+34.05)/2</f>
+        <v>34.33</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
@@ -1698,6 +1781,10 @@
       </c>
       <c r="H36" s="2" t="s">
         <v>143</v>
+      </c>
+      <c r="I36" s="1" t="n">
+        <f aca="false">(43.42+42)/2</f>
+        <v>42.71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>